<commit_message>
Updated table after adding a couple of PRS binaries
</commit_message>
<xml_diff>
--- a/tables/binary-neutron-stars-table.xlsx
+++ b/tables/binary-neutron-stars-table.xlsx
@@ -1,40 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alejandro/git/binary-neutron-stars-table/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338C6517-BB3E-6C48-8CD6-5FF826D904F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E9A71AE-3942-034E-8E3D-A4258A519D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19100" xr2:uid="{2E5B3542-A0DE-C34A-9F8C-AF3FC35586CA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19140"/>
   </bookViews>
   <sheets>
-    <sheet name="dummy_table" sheetId="1" r:id="rId1"/>
+    <sheet name="binary-neutron-stars-table" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="62">
   <si>
     <t>#</t>
   </si>
@@ -110,6 +96,75 @@
     </r>
   </si>
   <si>
+    <t>PSR B1913+16</t>
+  </si>
+  <si>
+    <t>PSR B2127+11C</t>
+  </si>
+  <si>
+    <t>PSR B1534+12</t>
+  </si>
+  <si>
+    <t>PSR J1518+4904</t>
+  </si>
+  <si>
+    <t>nan</t>
+  </si>
+  <si>
+    <t>PSR J1811-1736</t>
+  </si>
+  <si>
+    <t>PSR J0737-3039</t>
+  </si>
+  <si>
+    <t>PSR J1829+2456</t>
+  </si>
+  <si>
+    <t>PSR J1756-2251</t>
+  </si>
+  <si>
+    <t>PSR J1930-1852</t>
+  </si>
+  <si>
+    <t>PSR J0453+1559</t>
+  </si>
+  <si>
+    <t>PSR J1913+1102</t>
+  </si>
+  <si>
+    <t>GW170817</t>
+  </si>
+  <si>
+    <t>2,73-3,29</t>
+  </si>
+  <si>
+    <t>1,36-2,26</t>
+  </si>
+  <si>
+    <t>0,86-1,36</t>
+  </si>
+  <si>
+    <t>PSR J1411+2551</t>
+  </si>
+  <si>
+    <t>PSR J1757-1854</t>
+  </si>
+  <si>
+    <t>PSR J1946+2052</t>
+  </si>
+  <si>
+    <t>PSR J0509+3801</t>
+  </si>
+  <si>
+    <t>GW190425</t>
+  </si>
+  <si>
+    <t>1,60-2,52</t>
+  </si>
+  <si>
+    <t>1,12-1,69</t>
+  </si>
+  <si>
     <r>
       <t>P</t>
     </r>
@@ -173,13 +228,10 @@
     <t>Note</t>
   </si>
   <si>
-    <t>PSR B1913+16</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
-    <t>PSR B2127+11C</t>
+    <t>NA</t>
   </si>
   <si>
     <t>b</t>
@@ -188,134 +240,192 @@
     <t>*</t>
   </si>
   <si>
-    <t>PSR B1534+12</t>
-  </si>
-  <si>
     <t>c-d</t>
   </si>
   <si>
-    <t>PSR J1518+4904</t>
-  </si>
-  <si>
-    <t>nan</t>
-  </si>
-  <si>
     <t>inf</t>
   </si>
   <si>
     <t>e-f</t>
   </si>
   <si>
-    <t>PSR J1811-1736</t>
-  </si>
-  <si>
     <t>g-h</t>
   </si>
   <si>
-    <t>PSR J0737-3039</t>
-  </si>
-  <si>
     <t>i-j</t>
   </si>
   <si>
-    <t>PSR J1829+2456</t>
-  </si>
-  <si>
     <t>k</t>
   </si>
   <si>
-    <t>PSR J1756-2251</t>
-  </si>
-  <si>
     <t>l</t>
   </si>
   <si>
-    <t>PSR J1930-1852</t>
-  </si>
-  <si>
     <t>m</t>
   </si>
   <si>
-    <t>PSR J0453+1559</t>
-  </si>
-  <si>
     <t>n</t>
   </si>
   <si>
     <t>?</t>
   </si>
   <si>
-    <t>PSR J1913+1102</t>
-  </si>
-  <si>
-    <t>GW170817</t>
-  </si>
-  <si>
-    <t>2,73-3,29</t>
-  </si>
-  <si>
-    <t>1,36-2,26</t>
-  </si>
-  <si>
-    <t>0,86-1,36</t>
+    <t>o-p</t>
+  </si>
+  <si>
+    <t>q</t>
   </si>
   <si>
     <t>†</t>
   </si>
   <si>
-    <t>PSR J1411+2551</t>
-  </si>
-  <si>
-    <t>q</t>
-  </si>
-  <si>
-    <t>PSR J1757-1854</t>
-  </si>
-  <si>
     <t>r</t>
   </si>
   <si>
-    <t>PSR J0509+3801</t>
+    <t>s</t>
   </si>
   <si>
     <t>t</t>
   </si>
   <si>
-    <t>PSR J1946+2052</t>
-  </si>
-  <si>
-    <t>GW190425</t>
-  </si>
-  <si>
-    <t>1,60-2,52</t>
-  </si>
-  <si>
-    <t>1,12-1,69</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>o-p</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>u</t>
   </si>
   <si>
     <t>v</t>
+  </si>
+  <si>
+    <t>PSR J1759+5036</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>PSR J1753-2240</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -329,10 +439,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <vertAlign val="subscript"/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -345,16 +453,198 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <vertAlign val="subscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -362,19 +652,208 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="43">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -685,57 +1164,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11BB1569-DFF6-7A42-B506-C2CFA3B63DB0}">
-  <dimension ref="A1:M18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
+      <c r="G1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -743,7 +1219,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>1.2312000000000001</v>
@@ -769,14 +1245,14 @@
       <c r="J2">
         <v>301</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>14</v>
+      <c r="K2" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="L2">
         <v>1975</v>
       </c>
       <c r="M2" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -784,7 +1260,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>1.1805000000000001</v>
@@ -810,14 +1286,14 @@
       <c r="J3">
         <v>217</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>16</v>
+      <c r="K3" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="L3">
         <v>1990</v>
       </c>
       <c r="M3" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -825,7 +1301,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>1.1660999999999999</v>
@@ -852,13 +1328,13 @@
         <v>2739</v>
       </c>
       <c r="K4" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="L4">
         <v>1991</v>
       </c>
       <c r="M4" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -866,19 +1342,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D5">
         <v>2.718</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="G5">
         <v>40.9</v>
@@ -890,16 +1366,16 @@
         <v>0.249</v>
       </c>
       <c r="J5" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="K5" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="L5">
         <v>1997</v>
       </c>
       <c r="M5" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -907,19 +1383,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D6">
         <v>2.57</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="G6">
         <v>104.2</v>
@@ -931,16 +1407,16 @@
         <v>0.82799999999999996</v>
       </c>
       <c r="J6" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="K6" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="L6">
         <v>2001</v>
       </c>
       <c r="M6" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -948,7 +1424,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C7">
         <v>1.1253</v>
@@ -975,13 +1451,13 @@
         <v>86</v>
       </c>
       <c r="K7" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="L7">
         <v>2003</v>
       </c>
       <c r="M7" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -989,19 +1465,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D8">
         <v>2.59</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="G8">
         <v>41</v>
@@ -1013,16 +1489,16 @@
         <v>0.13900000000000001</v>
       </c>
       <c r="J8" t="s">
-        <v>22</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>29</v>
+        <v>41</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="L8">
         <v>2004</v>
       </c>
       <c r="M8" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -1030,7 +1506,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="C9">
         <v>1.1177999999999999</v>
@@ -1056,14 +1532,14 @@
       <c r="J9">
         <v>1663</v>
       </c>
-      <c r="K9" s="2" t="s">
-        <v>31</v>
+      <c r="K9" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="L9">
         <v>2005</v>
       </c>
       <c r="M9" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -1071,19 +1547,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D10">
         <v>2.59</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="G10">
         <v>185.5</v>
@@ -1095,16 +1571,16 @@
         <v>0.39900000000000002</v>
       </c>
       <c r="J10" t="s">
-        <v>22</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>33</v>
+        <v>41</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="L10">
         <v>2015</v>
       </c>
       <c r="M10" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -1112,7 +1588,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="C11">
         <v>1.1754</v>
@@ -1136,16 +1612,16 @@
         <v>0.113</v>
       </c>
       <c r="J11" t="s">
-        <v>22</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>35</v>
+        <v>41</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="L11">
         <v>2015</v>
       </c>
       <c r="M11" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -1153,7 +1629,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="C12">
         <v>1.2467999999999999</v>
@@ -1180,13 +1656,13 @@
         <v>470</v>
       </c>
       <c r="K12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="L12">
         <v>2016</v>
       </c>
       <c r="M12" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -1194,40 +1670,40 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="C13">
         <v>1.1879999999999999</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="E13" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="G13" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="H13" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="I13" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="J13" t="s">
-        <v>21</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>44</v>
+        <v>10</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="L13">
         <v>2017</v>
       </c>
       <c r="M13" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -1235,19 +1711,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D14">
         <v>2.5379999999999998</v>
       </c>
       <c r="E14" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="F14" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="G14">
         <v>62.4</v>
@@ -1259,16 +1735,16 @@
         <v>0.1699</v>
       </c>
       <c r="J14" t="s">
-        <v>22</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="L14">
         <v>2017</v>
       </c>
       <c r="M14" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -1276,7 +1752,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="C15">
         <v>1.1893</v>
@@ -1302,14 +1778,14 @@
       <c r="J15">
         <v>76</v>
       </c>
-      <c r="K15" s="2" t="s">
-        <v>55</v>
+      <c r="K15" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="L15">
         <v>2018</v>
       </c>
       <c r="M15" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -1317,19 +1793,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D16">
         <v>2.5</v>
       </c>
       <c r="E16" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="F16" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="G16">
         <v>17</v>
@@ -1343,14 +1819,14 @@
       <c r="J16">
         <v>46</v>
       </c>
-      <c r="K16" s="2" t="s">
-        <v>48</v>
+      <c r="K16" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="L16">
         <v>2018</v>
       </c>
       <c r="M16" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
@@ -1358,7 +1834,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="C17">
         <v>1.2174</v>
@@ -1384,14 +1860,14 @@
       <c r="J17">
         <v>580</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="K17" s="1" t="s">
         <v>56</v>
       </c>
       <c r="L17">
         <v>2018</v>
       </c>
       <c r="M17" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
@@ -1399,7 +1875,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="C18">
         <v>1.44</v>
@@ -1408,48 +1884,132 @@
         <v>3.4</v>
       </c>
       <c r="E18" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="F18" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="G18" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="H18" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="I18" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="J18" t="s">
-        <v>21</v>
-      </c>
-      <c r="K18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K18" s="1" t="s">
         <v>57</v>
       </c>
       <c r="L18">
         <v>2020</v>
       </c>
       <c r="M18" t="s">
-        <v>42</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19">
+        <v>2.62</v>
+      </c>
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19">
+        <v>176</v>
+      </c>
+      <c r="H19">
+        <v>2.04</v>
+      </c>
+      <c r="I19">
+        <v>0.3</v>
+      </c>
+      <c r="J19" t="s">
+        <v>41</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L19">
+        <v>2021</v>
+      </c>
+      <c r="M19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20">
+        <v>95.1</v>
+      </c>
+      <c r="H20">
+        <v>13.638</v>
+      </c>
+      <c r="I20">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="J20" t="s">
+        <v>41</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L20">
+        <v>2008</v>
+      </c>
+      <c r="M20" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" location="a" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - a" xr:uid="{6C71716C-2E5C-554A-B996-D96ABD83C560}"/>
-    <hyperlink ref="K3" r:id="rId2" location="b" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - b" xr:uid="{B400B9B6-3B75-4D4A-94D4-0308D6DFD883}"/>
-    <hyperlink ref="K8" r:id="rId3" location="k" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - k" xr:uid="{381C2148-6E70-D940-8CEA-4D08A4823330}"/>
-    <hyperlink ref="K9" r:id="rId4" location="l" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - l" xr:uid="{F8232852-95C4-3043-9FCA-CB32439DFEB8}"/>
-    <hyperlink ref="K10" r:id="rId5" location="m" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - m" xr:uid="{5192C7EF-7CC3-A847-9A63-2C3DB5C6AF7F}"/>
-    <hyperlink ref="K11" r:id="rId6" location="n" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - n" xr:uid="{1419B34B-5365-304E-A08A-82123167D107}"/>
-    <hyperlink ref="K13" r:id="rId7" location="q" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - q" xr:uid="{C02DBB0C-606E-6F49-AB08-997C9E245E4C}"/>
-    <hyperlink ref="K14" r:id="rId8" location="r" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - r" xr:uid="{8C7A64B5-C601-654B-B6EC-CA183D0836ED}"/>
-    <hyperlink ref="K15" r:id="rId9" location="s" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - s" xr:uid="{E2A375C0-9CFF-AC47-A4B8-CB4F77F619CC}"/>
-    <hyperlink ref="K16" r:id="rId10" location="t" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - t" xr:uid="{03FB2339-C0E7-6044-B9DE-7CCA7E3C19AC}"/>
-    <hyperlink ref="K17" r:id="rId11" location="u" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - u" xr:uid="{D3E2582C-2583-C042-B554-DCF736A0740A}"/>
-    <hyperlink ref="K18" r:id="rId12" location="v" display="https://github.com/avigna/binary-neutron-stars-table/blob/main/README.md - v" xr:uid="{7636458B-7E16-8E45-A27B-E5AEDC45BE5A}"/>
+    <hyperlink ref="K2" r:id="rId1" location="a" display="https://github.com/avigna/binary-neutron-stars-table - a"/>
+    <hyperlink ref="K3" r:id="rId2" location="b" display="https://github.com/avigna/binary-neutron-stars-table - b"/>
+    <hyperlink ref="K8" r:id="rId3" location="k" display="https://github.com/avigna/binary-neutron-stars-table - k"/>
+    <hyperlink ref="K9" r:id="rId4" location="l" display="https://github.com/avigna/binary-neutron-stars-table - l"/>
+    <hyperlink ref="K10" r:id="rId5" location="m" display="https://github.com/avigna/binary-neutron-stars-table - m"/>
+    <hyperlink ref="K11" r:id="rId6" location="n" display="https://github.com/avigna/binary-neutron-stars-table - n"/>
+    <hyperlink ref="K13" r:id="rId7" location="q" display="https://github.com/avigna/binary-neutron-stars-table - q"/>
+    <hyperlink ref="K14" r:id="rId8" location="r" display="https://github.com/avigna/binary-neutron-stars-table - r"/>
+    <hyperlink ref="K15" r:id="rId9" location="s" display="https://github.com/avigna/binary-neutron-stars-table - s"/>
+    <hyperlink ref="K16" r:id="rId10" location="t" display="https://github.com/avigna/binary-neutron-stars-table - t"/>
+    <hyperlink ref="K17" r:id="rId11" location="u" display="https://github.com/avigna/binary-neutron-stars-table - u"/>
+    <hyperlink ref="K18" r:id="rId12" location="v" display="https://github.com/avigna/binary-neutron-stars-table - v"/>
+    <hyperlink ref="K19" r:id="rId13" location="w" display="https://github.com/avigna/binary-neutron-stars-table - w"/>
+    <hyperlink ref="K20" r:id="rId14" location="x" display="https://github.com/avigna/binary-neutron-stars-table - x"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>